<commit_message>
Steffens tidsregistrering fra den 8/3
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering Steffen.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering Steffen.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -208,6 +208,18 @@
   </si>
   <si>
     <t>Brugertests</t>
+  </si>
+  <si>
+    <t>krydstjek</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>spørgsmål</t>
+  </si>
+  <si>
+    <t>OC 1-3-4</t>
   </si>
 </sst>
 </file>
@@ -261,10 +273,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,7 +594,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,17 +610,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
@@ -660,10 +672,10 @@
       <c r="F5" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>0.35416666666666669</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>0.64583333333333337</v>
       </c>
       <c r="I5">
@@ -675,10 +687,10 @@
       <c r="F6" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>0.54166666666666663</v>
       </c>
       <c r="I6">
@@ -687,17 +699,19 @@
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <v>42801</v>
+      </c>
       <c r="E7" t="s">
         <v>3</v>
       </c>
       <c r="F7" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>0.35416666666666669</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>0.4375</v>
       </c>
       <c r="I7">
@@ -712,10 +726,10 @@
       <c r="F8" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>0.4375</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>0.64583333333333337</v>
       </c>
       <c r="I8">
@@ -726,19 +740,69 @@
       <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1">
+        <v>42802</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.34375</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
+      <c r="F13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
+      <c r="F14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>

</xml_diff>

<commit_message>
tidsregistering, skulle nok have udfyldt det løbende
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering Steffen.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering Steffen.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="75">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -247,6 +247,15 @@
   </si>
   <si>
     <t>design OC5</t>
+  </si>
+  <si>
+    <t>bugfixing</t>
+  </si>
+  <si>
+    <t>gui - bugfixing</t>
+  </si>
+  <si>
+    <t>design</t>
   </si>
 </sst>
 </file>
@@ -618,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,6 +987,134 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>42810</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>42814</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
+        <v>74</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="H40" s="5">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I40" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>42815</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>69</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>42816</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F47" t="s">
+        <v>69</v>
+      </c>
+      <c r="G47" s="5">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="H47" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I47">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F48" t="s">
+        <v>72</v>
+      </c>
+      <c r="G48" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H48" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>42817</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F51" t="s">
+        <v>73</v>
+      </c>
+      <c r="G51" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H51" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F52" t="s">
+        <v>69</v>
+      </c>
+      <c r="G52" s="5">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="H52" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>42818</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F55" t="s">
+        <v>73</v>
+      </c>
+      <c r="G55" s="5">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="H55" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="I55">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>